<commit_message>
ExcelReaderTest and ArgumentsParserTest now pass and their errors have been fixed
</commit_message>
<xml_diff>
--- a/src/test/resources/test.xlsx
+++ b/src/test/resources/test.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documentos\Uni\ASW\practicas\trabajos\1er trabajo\censuses_i1a\src\test\resources\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="8370" windowHeight="2370"/>
   </bookViews>
@@ -16,9 +21,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
-    <t>Nombre</t>
-  </si>
-  <si>
     <t>NIF</t>
   </si>
   <si>
@@ -53,6 +55,9 @@
   </si>
   <si>
     <t>anita87@gmail.com</t>
+  </si>
+  <si>
+    <t>Name</t>
   </si>
 </sst>
 </file>
@@ -133,6 +138,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -393,7 +401,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -403,9 +411,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -415,27 +421,27 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
       <c r="C1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D1" t="s">
         <v>8</v>
-      </c>
-      <c r="D1" t="s">
-        <v>9</v>
       </c>
     </row>
     <row r="2" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D2">
         <v>1</v>
@@ -443,13 +449,13 @@
     </row>
     <row r="3" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" t="s">
         <v>4</v>
       </c>
-      <c r="B3" t="s">
-        <v>5</v>
-      </c>
       <c r="C3" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D3">
         <v>2</v>
@@ -457,13 +463,13 @@
     </row>
     <row r="4" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="1" t="s">
-        <v>7</v>
-      </c>
       <c r="C4" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D4">
         <v>2</v>

</xml_diff>